<commit_message>
- lodash - 多语言
</commit_message>
<xml_diff>
--- a/tools/config.xlsx
+++ b/tools/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="12660"/>
+    <workbookView windowWidth="24940" windowHeight="12660"/>
   </bookViews>
   <sheets>
     <sheet name="loading-language" sheetId="1" r:id="rId1"/>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF067D17"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
       <t>所有资源加载完成，进入主场景</t>
     </r>
     <r>
@@ -66,6 +72,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF067D17"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
       <t>正在检查资源，并准备热梗</t>
     </r>
     <r>
@@ -101,7 +113,7 @@
     <t>ui_loading_loading_dir</t>
   </si>
   <si>
-    <t>Loading directory: ${dir}......</t>
+    <t>Loading directory: %{dir}......</t>
   </si>
   <si>
     <r>
@@ -109,17 +121,37 @@
     </r>
     <r>
       <rPr>
-        <sz val="9.8"/>
+        <sz val="10"/>
         <color rgb="FF080808"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>%{dir}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF067D17"/>
         <rFont val="宋体"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>${</t>
+      <t>......</t>
+    </r>
+  </si>
+  <si>
+    <t>ui_loading_loading_done</t>
+  </si>
+  <si>
+    <t>%{dir} loading complete</t>
+  </si>
+  <si>
+    <r>
+      <t>%{</t>
     </r>
     <r>
       <rPr>
-        <sz val="9.8"/>
+        <sz val="10"/>
         <color rgb="FF2A8C7C"/>
         <rFont val="宋体"/>
         <charset val="134"/>
@@ -129,48 +161,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="9.8"/>
-        <color rgb="FF080808"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8"/>
-        <color rgb="FF067D17"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>......</t>
-    </r>
-  </si>
-  <si>
-    <t>ui_loading_loading_done</t>
-  </si>
-  <si>
-    <t>${dir} loading complete</t>
-  </si>
-  <si>
-    <r>
-      <t>${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8"/>
-        <color rgb="FF2A8C7C"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dir</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8"/>
+        <sz val="10"/>
         <color rgb="FF080808"/>
         <rFont val="宋体"/>
         <charset val="134"/>
@@ -180,7 +171,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="9.8"/>
+        <sz val="10"/>
         <color rgb="FF067D17"/>
         <rFont val="宋体"/>
         <charset val="134"/>
@@ -200,7 +191,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,7 +212,13 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9.8"/>
+      <sz val="10"/>
+      <color rgb="FF067D17"/>
+      <name val="宋体-简"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF080808"/>
       <name val="Courier New"/>
       <charset val="134"/>
@@ -371,22 +368,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF2A8C7C"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF080808"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF067D17"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9.8"/>
       <color rgb="FF067D17"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9.8"/>
-      <color rgb="FF2A8C7C"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9.8"/>
-      <color rgb="FF080808"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -712,137 +716,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -853,6 +857,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1383,7 +1390,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A3" sqref="$A3:$XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="2"/>
@@ -1455,7 +1462,7 @@
       <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1466,7 +1473,7 @@
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>